<commit_message>
rajout lien vers 3 pages html vierge
</commit_message>
<xml_diff>
--- a/planning_projet.xlsx
+++ b/planning_projet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\synow\jess\ADA\travailCollectifAda\dataviz\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\synow\jess\ADA\travailCollectifAda\dataviz\le_trio-gourmet_jay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95DB976D-7DCB-4436-BDA7-DBEEBD52DA95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66948B9A-787E-4EF2-BC0C-5DFAF19B245C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{67D91FEB-0FE5-4B90-85E5-6BCC547C0F94}"/>
+    <workbookView xWindow="2100" yWindow="4110" windowWidth="19200" windowHeight="11170" xr2:uid="{67D91FEB-0FE5-4B90-85E5-6BCC547C0F94}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Suivi projet dataviz -Auguste/yohan/jess</t>
   </si>
@@ -60,7 +60,16 @@
     <t>ok</t>
   </si>
   <si>
-    <t>faire le css</t>
+    <t>auguste: filtrer par nom</t>
+  </si>
+  <si>
+    <t>yohan: filtrer par ingredient</t>
+  </si>
+  <si>
+    <t>jess: filtrer par pays</t>
+  </si>
+  <si>
+    <t>faire le css page d accueil</t>
   </si>
 </sst>
 </file>
@@ -432,7 +441,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -484,23 +493,33 @@
         <v>45006</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>45010</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>